<commit_message>
images and statistics added
</commit_message>
<xml_diff>
--- a/data/results/dritter_durchlauf/statistics.xlsx
+++ b/data/results/dritter_durchlauf/statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Bachelorarbeit\Code\bachelorthesis\data\results\dritter_durchlauf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445865C1-64AE-4312-B135-B9D3D53F27CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693D5F61-476A-4280-A55F-3630F6E4274F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="41115" yWindow="7785" windowWidth="16080" windowHeight="13440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>Methode</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>0.767</t>
+  </si>
+  <si>
+    <t>0.81</t>
+  </si>
+  <si>
+    <t>0.977</t>
   </si>
 </sst>
 </file>
@@ -428,7 +434,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:F12"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,7 +484,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1">
-        <v>0.97</v>
+        <v>0.97199999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -498,7 +504,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.57799999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -518,7 +524,7 @@
         <v>0.81</v>
       </c>
       <c r="F4" s="1">
-        <v>0.72</v>
+        <v>0.72499999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -528,10 +534,18 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -540,10 +554,18 @@
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.70099999999999996</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -552,10 +574,18 @@
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="C7" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.45800000000000002</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">

</xml_diff>